<commit_message>
updae log , add 439
</commit_message>
<xml_diff>
--- a/pythonProject1/LeetcodeDaylog.xlsx
+++ b/pythonProject1/LeetcodeDaylog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mingzhu\PycharmProjects\pythonProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112EE33-AF93-45F6-8AE8-5C92F2A17023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F026A-2E95-44AC-A155-C3E76711B533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>date\level</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -74,11 +82,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -360,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -371,7 +380,10 @@
     <col min="1" max="1" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2">
         <v>3</v>
       </c>
@@ -379,88 +391,144 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="3">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="3">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44650</v>
       </c>
       <c r="B2">
         <v>439</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>1003</v>
+      </c>
+      <c r="D2">
+        <v>388</v>
+      </c>
+      <c r="E2">
+        <v>735</v>
+      </c>
+      <c r="F2">
+        <v>962</v>
+      </c>
+      <c r="G2">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44651</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1910</v>
+      </c>
+      <c r="C3">
+        <v>1047</v>
+      </c>
+      <c r="D3">
+        <v>496</v>
+      </c>
+      <c r="E3">
+        <v>962</v>
+      </c>
+      <c r="F3">
+        <v>901</v>
+      </c>
+      <c r="G3">
+        <v>402</v>
+      </c>
+      <c r="H3">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44652</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>739</v>
+      </c>
+      <c r="C4">
+        <v>1229</v>
+      </c>
+      <c r="D4">
+        <v>1305</v>
+      </c>
+      <c r="E4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44653</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44654</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44655</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44656</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44657</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44658</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44659</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44660</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44661</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44662</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44663</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44664</v>
       </c>
@@ -560,7 +628,28 @@
         <v>44683</v>
       </c>
     </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>44685</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>44686</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>44687</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>